<commit_message>
updated dataset from brasil.io
</commit_message>
<xml_diff>
--- a/assets/Helper_SP.xlsx
+++ b/assets/Helper_SP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\andre\Task Stage\Task - covidsims\covidsims\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08241548-0D85-43A3-949F-A29560659C9C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C5C8E7-FCE8-4BB5-86D0-70D838C05AD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="16440" tabRatio="659" activeTab="2" xr2:uid="{C9EED678-3558-4294-B636-EA4BD58922A2}"/>
+    <workbookView xWindow="20370" yWindow="-120" windowWidth="38640" windowHeight="16440" tabRatio="659" xr2:uid="{C9EED678-3558-4294-B636-EA4BD58922A2}"/>
   </bookViews>
   <sheets>
     <sheet name="dados_diarios_estado_SP" sheetId="7" r:id="rId1"/>
@@ -278,6 +278,1403 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>daily_changes!$F$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>∆C(t)</c:v>
+                </c:pt>
+              </c:strCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="31750" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>daily_changes!$F$2:$F$452</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="451"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>35</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>49</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>56</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>85</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>92</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>89</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>109</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>118</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>135</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>117</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>110</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>218</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>303</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>351</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>404</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>437</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>453</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>478</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>532</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>568</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>595</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>565</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>591</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>576</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>527</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>619</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>584</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>661</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>782</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>787</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>812</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>859</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>696</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>739</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>712</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>873</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>921</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>1017</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>1237</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1463</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>1708</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>1793</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>1596</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>1580</c:v>
+                </c:pt>
+                <c:pt idx="69">
+                  <c:v>1499</c:v>
+                </c:pt>
+                <c:pt idx="70">
+                  <c:v>1430</c:v>
+                </c:pt>
+                <c:pt idx="71">
+                  <c:v>1671</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1604</c:v>
+                </c:pt>
+                <c:pt idx="73">
+                  <c:v>1637</c:v>
+                </c:pt>
+                <c:pt idx="74">
+                  <c:v>1891</c:v>
+                </c:pt>
+                <c:pt idx="75">
+                  <c:v>1953</c:v>
+                </c:pt>
+                <c:pt idx="76">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="77">
+                  <c:v>1952</c:v>
+                </c:pt>
+                <c:pt idx="78">
+                  <c:v>1892</c:v>
+                </c:pt>
+                <c:pt idx="79">
+                  <c:v>2051</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>2364</c:v>
+                </c:pt>
+                <c:pt idx="81">
+                  <c:v>2396</c:v>
+                </c:pt>
+                <c:pt idx="82">
+                  <c:v>2414</c:v>
+                </c:pt>
+                <c:pt idx="83">
+                  <c:v>2419</c:v>
+                </c:pt>
+                <c:pt idx="84">
+                  <c:v>2611</c:v>
+                </c:pt>
+                <c:pt idx="85">
+                  <c:v>2680</c:v>
+                </c:pt>
+                <c:pt idx="86">
+                  <c:v>2779</c:v>
+                </c:pt>
+                <c:pt idx="87">
+                  <c:v>2642</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>2768</c:v>
+                </c:pt>
+                <c:pt idx="89">
+                  <c:v>2831</c:v>
+                </c:pt>
+                <c:pt idx="90">
+                  <c:v>2937</c:v>
+                </c:pt>
+                <c:pt idx="91">
+                  <c:v>2860</c:v>
+                </c:pt>
+                <c:pt idx="92">
+                  <c:v>2803</c:v>
+                </c:pt>
+                <c:pt idx="93">
+                  <c:v>3161</c:v>
+                </c:pt>
+                <c:pt idx="94">
+                  <c:v>3526</c:v>
+                </c:pt>
+                <c:pt idx="95">
+                  <c:v>3798</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>3934</c:v>
+                </c:pt>
+                <c:pt idx="97">
+                  <c:v>3953</c:v>
+                </c:pt>
+                <c:pt idx="98">
+                  <c:v>4611</c:v>
+                </c:pt>
+                <c:pt idx="99">
+                  <c:v>4857</c:v>
+                </c:pt>
+                <c:pt idx="100">
+                  <c:v>4762</c:v>
+                </c:pt>
+                <c:pt idx="101">
+                  <c:v>4716</c:v>
+                </c:pt>
+                <c:pt idx="102">
+                  <c:v>4772</c:v>
+                </c:pt>
+                <c:pt idx="103">
+                  <c:v>4768</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>4757</c:v>
+                </c:pt>
+                <c:pt idx="105">
+                  <c:v>4549</c:v>
+                </c:pt>
+                <c:pt idx="106">
+                  <c:v>4690</c:v>
+                </c:pt>
+                <c:pt idx="107">
+                  <c:v>4760</c:v>
+                </c:pt>
+                <c:pt idx="108">
+                  <c:v>4762</c:v>
+                </c:pt>
+                <c:pt idx="109">
+                  <c:v>4618</c:v>
+                </c:pt>
+                <c:pt idx="110">
+                  <c:v>5018</c:v>
+                </c:pt>
+                <c:pt idx="111">
+                  <c:v>5267</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>5735</c:v>
+                </c:pt>
+                <c:pt idx="113">
+                  <c:v>5029</c:v>
+                </c:pt>
+                <c:pt idx="114">
+                  <c:v>4301</c:v>
+                </c:pt>
+                <c:pt idx="115">
+                  <c:v>6251</c:v>
+                </c:pt>
+                <c:pt idx="116">
+                  <c:v>6131</c:v>
+                </c:pt>
+                <c:pt idx="117">
+                  <c:v>5855</c:v>
+                </c:pt>
+                <c:pt idx="118">
+                  <c:v>5788</c:v>
+                </c:pt>
+                <c:pt idx="119">
+                  <c:v>5599</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>6758</c:v>
+                </c:pt>
+                <c:pt idx="121">
+                  <c:v>7994</c:v>
+                </c:pt>
+                <c:pt idx="122">
+                  <c:v>6693</c:v>
+                </c:pt>
+                <c:pt idx="123">
+                  <c:v>7113</c:v>
+                </c:pt>
+                <c:pt idx="124">
+                  <c:v>7507</c:v>
+                </c:pt>
+                <c:pt idx="125">
+                  <c:v>7596</c:v>
+                </c:pt>
+                <c:pt idx="126">
+                  <c:v>7415</c:v>
+                </c:pt>
+                <c:pt idx="127">
+                  <c:v>7302</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>7656</c:v>
+                </c:pt>
+                <c:pt idx="129">
+                  <c:v>7456</c:v>
+                </c:pt>
+                <c:pt idx="130">
+                  <c:v>6707</c:v>
+                </c:pt>
+                <c:pt idx="131">
+                  <c:v>6920</c:v>
+                </c:pt>
+                <c:pt idx="132">
+                  <c:v>6846</c:v>
+                </c:pt>
+                <c:pt idx="133">
+                  <c:v>7333</c:v>
+                </c:pt>
+                <c:pt idx="134">
+                  <c:v>7347</c:v>
+                </c:pt>
+                <c:pt idx="135">
+                  <c:v>6791</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>6915</c:v>
+                </c:pt>
+                <c:pt idx="137">
+                  <c:v>7766</c:v>
+                </c:pt>
+                <c:pt idx="138">
+                  <c:v>7403</c:v>
+                </c:pt>
+                <c:pt idx="139">
+                  <c:v>7362</c:v>
+                </c:pt>
+                <c:pt idx="140">
+                  <c:v>7700</c:v>
+                </c:pt>
+                <c:pt idx="141">
+                  <c:v>7402</c:v>
+                </c:pt>
+                <c:pt idx="142">
+                  <c:v>7476</c:v>
+                </c:pt>
+                <c:pt idx="143">
+                  <c:v>6901</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>6448</c:v>
+                </c:pt>
+                <c:pt idx="145">
+                  <c:v>6150</c:v>
+                </c:pt>
+                <c:pt idx="146">
+                  <c:v>5975</c:v>
+                </c:pt>
+                <c:pt idx="147">
+                  <c:v>5152</c:v>
+                </c:pt>
+                <c:pt idx="148">
+                  <c:v>6610</c:v>
+                </c:pt>
+                <c:pt idx="149">
+                  <c:v>7137</c:v>
+                </c:pt>
+                <c:pt idx="150">
+                  <c:v>7972</c:v>
+                </c:pt>
+                <c:pt idx="151">
+                  <c:v>9636</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>9848</c:v>
+                </c:pt>
+                <c:pt idx="153">
+                  <c:v>10174</c:v>
+                </c:pt>
+                <c:pt idx="154">
+                  <c:v>9284</c:v>
+                </c:pt>
+                <c:pt idx="155">
+                  <c:v>10679</c:v>
+                </c:pt>
+                <c:pt idx="156">
+                  <c:v>11000</c:v>
+                </c:pt>
+                <c:pt idx="157">
+                  <c:v>11298</c:v>
+                </c:pt>
+                <c:pt idx="158">
+                  <c:v>10405</c:v>
+                </c:pt>
+                <c:pt idx="159">
+                  <c:v>10672</c:v>
+                </c:pt>
+                <c:pt idx="160">
+                  <c:v>10366</c:v>
+                </c:pt>
+                <c:pt idx="161">
+                  <c:v>12562</c:v>
+                </c:pt>
+                <c:pt idx="162">
+                  <c:v>10153</c:v>
+                </c:pt>
+                <c:pt idx="163">
+                  <c:v>9952</c:v>
+                </c:pt>
+                <c:pt idx="164">
+                  <c:v>9439</c:v>
+                </c:pt>
+                <c:pt idx="165">
+                  <c:v>9916</c:v>
+                </c:pt>
+                <c:pt idx="166">
+                  <c:v>9777</c:v>
+                </c:pt>
+                <c:pt idx="167">
+                  <c:v>9742</c:v>
+                </c:pt>
+                <c:pt idx="168">
+                  <c:v>9139</c:v>
+                </c:pt>
+                <c:pt idx="169">
+                  <c:v>9988</c:v>
+                </c:pt>
+                <c:pt idx="170">
+                  <c:v>10826</c:v>
+                </c:pt>
+                <c:pt idx="171">
+                  <c:v>11106</c:v>
+                </c:pt>
+                <c:pt idx="172">
+                  <c:v>10828</c:v>
+                </c:pt>
+                <c:pt idx="173">
+                  <c:v>10338</c:v>
+                </c:pt>
+                <c:pt idx="174">
+                  <c:v>10607</c:v>
+                </c:pt>
+                <c:pt idx="175">
+                  <c:v>10281</c:v>
+                </c:pt>
+                <c:pt idx="176">
+                  <c:v>9457</c:v>
+                </c:pt>
+                <c:pt idx="177">
+                  <c:v>8053</c:v>
+                </c:pt>
+                <c:pt idx="178">
+                  <c:v>7120</c:v>
+                </c:pt>
+                <c:pt idx="179">
+                  <c:v>7388</c:v>
+                </c:pt>
+                <c:pt idx="180">
+                  <c:v>7805</c:v>
+                </c:pt>
+                <c:pt idx="181">
+                  <c:v>7688</c:v>
+                </c:pt>
+                <c:pt idx="182">
+                  <c:v>7734</c:v>
+                </c:pt>
+                <c:pt idx="183">
+                  <c:v>7823</c:v>
+                </c:pt>
+                <c:pt idx="184">
+                  <c:v>7661</c:v>
+                </c:pt>
+                <c:pt idx="185">
+                  <c:v>8607</c:v>
+                </c:pt>
+                <c:pt idx="186">
+                  <c:v>7454</c:v>
+                </c:pt>
+                <c:pt idx="187">
+                  <c:v>7039</c:v>
+                </c:pt>
+                <c:pt idx="188">
+                  <c:v>6837</c:v>
+                </c:pt>
+                <c:pt idx="189">
+                  <c:v>6958</c:v>
+                </c:pt>
+                <c:pt idx="190">
+                  <c:v>7171</c:v>
+                </c:pt>
+                <c:pt idx="191">
+                  <c:v>7646</c:v>
+                </c:pt>
+                <c:pt idx="192">
+                  <c:v>6972</c:v>
+                </c:pt>
+                <c:pt idx="193">
+                  <c:v>7380</c:v>
+                </c:pt>
+                <c:pt idx="194">
+                  <c:v>7474</c:v>
+                </c:pt>
+                <c:pt idx="195">
+                  <c:v>7570</c:v>
+                </c:pt>
+                <c:pt idx="196">
+                  <c:v>6344</c:v>
+                </c:pt>
+                <c:pt idx="197">
+                  <c:v>5749</c:v>
+                </c:pt>
+                <c:pt idx="198">
+                  <c:v>5254</c:v>
+                </c:pt>
+                <c:pt idx="199">
+                  <c:v>5399</c:v>
+                </c:pt>
+                <c:pt idx="200">
+                  <c:v>5372</c:v>
+                </c:pt>
+                <c:pt idx="201">
+                  <c:v>5219</c:v>
+                </c:pt>
+                <c:pt idx="202">
+                  <c:v>5146</c:v>
+                </c:pt>
+                <c:pt idx="203">
+                  <c:v>6070</c:v>
+                </c:pt>
+                <c:pt idx="204">
+                  <c:v>6122</c:v>
+                </c:pt>
+                <c:pt idx="205">
+                  <c:v>6010</c:v>
+                </c:pt>
+                <c:pt idx="206">
+                  <c:v>5960</c:v>
+                </c:pt>
+                <c:pt idx="207">
+                  <c:v>5855</c:v>
+                </c:pt>
+                <c:pt idx="208">
+                  <c:v>6149</c:v>
+                </c:pt>
+                <c:pt idx="209">
+                  <c:v>6283</c:v>
+                </c:pt>
+                <c:pt idx="210">
+                  <c:v>6307</c:v>
+                </c:pt>
+                <c:pt idx="211">
+                  <c:v>6078</c:v>
+                </c:pt>
+                <c:pt idx="212">
+                  <c:v>5917</c:v>
+                </c:pt>
+                <c:pt idx="213">
+                  <c:v>5770</c:v>
+                </c:pt>
+                <c:pt idx="214">
+                  <c:v>5602</c:v>
+                </c:pt>
+                <c:pt idx="215">
+                  <c:v>5277</c:v>
+                </c:pt>
+                <c:pt idx="216">
+                  <c:v>5116</c:v>
+                </c:pt>
+                <c:pt idx="217">
+                  <c:v>4871</c:v>
+                </c:pt>
+                <c:pt idx="218">
+                  <c:v>4808</c:v>
+                </c:pt>
+                <c:pt idx="219">
+                  <c:v>4784</c:v>
+                </c:pt>
+                <c:pt idx="220">
+                  <c:v>4630</c:v>
+                </c:pt>
+                <c:pt idx="221">
+                  <c:v>4649</c:v>
+                </c:pt>
+                <c:pt idx="222">
+                  <c:v>4524</c:v>
+                </c:pt>
+                <c:pt idx="223">
+                  <c:v>4491</c:v>
+                </c:pt>
+                <c:pt idx="224">
+                  <c:v>4474</c:v>
+                </c:pt>
+                <c:pt idx="225">
+                  <c:v>4447</c:v>
+                </c:pt>
+                <c:pt idx="226">
+                  <c:v>4383</c:v>
+                </c:pt>
+                <c:pt idx="227">
+                  <c:v>4408</c:v>
+                </c:pt>
+                <c:pt idx="228">
+                  <c:v>4484</c:v>
+                </c:pt>
+                <c:pt idx="229">
+                  <c:v>4823</c:v>
+                </c:pt>
+                <c:pt idx="230">
+                  <c:v>4824</c:v>
+                </c:pt>
+                <c:pt idx="231">
+                  <c:v>4027</c:v>
+                </c:pt>
+                <c:pt idx="232">
+                  <c:v>4044</c:v>
+                </c:pt>
+                <c:pt idx="233">
+                  <c:v>4173</c:v>
+                </c:pt>
+                <c:pt idx="234">
+                  <c:v>4150</c:v>
+                </c:pt>
+                <c:pt idx="235">
+                  <c:v>3974</c:v>
+                </c:pt>
+                <c:pt idx="236">
+                  <c:v>3706</c:v>
+                </c:pt>
+                <c:pt idx="237">
+                  <c:v>3671</c:v>
+                </c:pt>
+                <c:pt idx="238">
+                  <c:v>4276</c:v>
+                </c:pt>
+                <c:pt idx="239">
+                  <c:v>4029</c:v>
+                </c:pt>
+                <c:pt idx="240">
+                  <c:v>3618</c:v>
+                </c:pt>
+                <c:pt idx="241">
+                  <c:v>3772</c:v>
+                </c:pt>
+                <c:pt idx="242">
+                  <c:v>3803</c:v>
+                </c:pt>
+                <c:pt idx="243">
+                  <c:v>4054</c:v>
+                </c:pt>
+                <c:pt idx="244">
+                  <c:v>4115</c:v>
+                </c:pt>
+                <c:pt idx="245">
+                  <c:v>4178</c:v>
+                </c:pt>
+                <c:pt idx="246">
+                  <c:v>4332</c:v>
+                </c:pt>
+                <c:pt idx="247">
+                  <c:v>4560</c:v>
+                </c:pt>
+                <c:pt idx="248">
+                  <c:v>4307</c:v>
+                </c:pt>
+                <c:pt idx="249">
+                  <c:v>3839</c:v>
+                </c:pt>
+                <c:pt idx="250">
+                  <c:v>3595</c:v>
+                </c:pt>
+                <c:pt idx="251">
+                  <c:v>3565</c:v>
+                </c:pt>
+                <c:pt idx="252">
+                  <c:v>2905</c:v>
+                </c:pt>
+                <c:pt idx="253">
+                  <c:v>2817</c:v>
+                </c:pt>
+                <c:pt idx="254">
+                  <c:v>2439</c:v>
+                </c:pt>
+                <c:pt idx="255">
+                  <c:v>1735</c:v>
+                </c:pt>
+                <c:pt idx="256">
+                  <c:v>1401</c:v>
+                </c:pt>
+                <c:pt idx="257">
+                  <c:v>1256</c:v>
+                </c:pt>
+                <c:pt idx="258">
+                  <c:v>1163</c:v>
+                </c:pt>
+                <c:pt idx="259">
+                  <c:v>1056</c:v>
+                </c:pt>
+                <c:pt idx="260">
+                  <c:v>3939</c:v>
+                </c:pt>
+                <c:pt idx="261">
+                  <c:v>4388</c:v>
+                </c:pt>
+                <c:pt idx="262">
+                  <c:v>5264</c:v>
+                </c:pt>
+                <c:pt idx="263">
+                  <c:v>5927</c:v>
+                </c:pt>
+                <c:pt idx="264">
+                  <c:v>6101</c:v>
+                </c:pt>
+                <c:pt idx="265">
+                  <c:v>6206</c:v>
+                </c:pt>
+                <c:pt idx="266">
+                  <c:v>7448</c:v>
+                </c:pt>
+                <c:pt idx="267">
+                  <c:v>4803</c:v>
+                </c:pt>
+                <c:pt idx="268">
+                  <c:v>4948</c:v>
+                </c:pt>
+                <c:pt idx="269">
+                  <c:v>5367</c:v>
+                </c:pt>
+                <c:pt idx="270">
+                  <c:v>5430</c:v>
+                </c:pt>
+                <c:pt idx="271">
+                  <c:v>5850</c:v>
+                </c:pt>
+                <c:pt idx="272">
+                  <c:v>5893</c:v>
+                </c:pt>
+                <c:pt idx="273">
+                  <c:v>5396</c:v>
+                </c:pt>
+                <c:pt idx="274">
+                  <c:v>5750</c:v>
+                </c:pt>
+                <c:pt idx="275">
+                  <c:v>5425</c:v>
+                </c:pt>
+                <c:pt idx="276">
+                  <c:v>4748</c:v>
+                </c:pt>
+                <c:pt idx="277">
+                  <c:v>4666</c:v>
+                </c:pt>
+                <c:pt idx="278">
+                  <c:v>4412</c:v>
+                </c:pt>
+                <c:pt idx="279">
+                  <c:v>4433</c:v>
+                </c:pt>
+                <c:pt idx="280">
+                  <c:v>4964</c:v>
+                </c:pt>
+                <c:pt idx="281">
+                  <c:v>4994</c:v>
+                </c:pt>
+                <c:pt idx="282">
+                  <c:v>5521</c:v>
+                </c:pt>
+                <c:pt idx="283">
+                  <c:v>6080</c:v>
+                </c:pt>
+                <c:pt idx="284">
+                  <c:v>6713</c:v>
+                </c:pt>
+                <c:pt idx="285">
+                  <c:v>6756</c:v>
+                </c:pt>
+                <c:pt idx="286">
+                  <c:v>6746</c:v>
+                </c:pt>
+                <c:pt idx="287">
+                  <c:v>6602</c:v>
+                </c:pt>
+                <c:pt idx="288">
+                  <c:v>6697</c:v>
+                </c:pt>
+                <c:pt idx="289">
+                  <c:v>6923</c:v>
+                </c:pt>
+                <c:pt idx="290">
+                  <c:v>7002</c:v>
+                </c:pt>
+                <c:pt idx="291">
+                  <c:v>6954</c:v>
+                </c:pt>
+                <c:pt idx="292">
+                  <c:v>6706</c:v>
+                </c:pt>
+                <c:pt idx="293">
+                  <c:v>6877</c:v>
+                </c:pt>
+                <c:pt idx="294">
+                  <c:v>6375</c:v>
+                </c:pt>
+                <c:pt idx="295">
+                  <c:v>4978</c:v>
+                </c:pt>
+                <c:pt idx="296">
+                  <c:v>6480</c:v>
+                </c:pt>
+                <c:pt idx="297">
+                  <c:v>6642</c:v>
+                </c:pt>
+                <c:pt idx="298">
+                  <c:v>7191</c:v>
+                </c:pt>
+                <c:pt idx="299">
+                  <c:v>7057</c:v>
+                </c:pt>
+                <c:pt idx="300">
+                  <c:v>7290</c:v>
+                </c:pt>
+                <c:pt idx="301">
+                  <c:v>8190</c:v>
+                </c:pt>
+                <c:pt idx="302">
+                  <c:v>9673</c:v>
+                </c:pt>
+                <c:pt idx="303">
+                  <c:v>8109</c:v>
+                </c:pt>
+                <c:pt idx="304">
+                  <c:v>7205</c:v>
+                </c:pt>
+                <c:pt idx="305">
+                  <c:v>5606</c:v>
+                </c:pt>
+                <c:pt idx="306">
+                  <c:v>6011</c:v>
+                </c:pt>
+                <c:pt idx="307">
+                  <c:v>5673</c:v>
+                </c:pt>
+                <c:pt idx="308">
+                  <c:v>5925</c:v>
+                </c:pt>
+                <c:pt idx="309">
+                  <c:v>6134</c:v>
+                </c:pt>
+                <c:pt idx="310">
+                  <c:v>6258</c:v>
+                </c:pt>
+                <c:pt idx="311">
+                  <c:v>6301</c:v>
+                </c:pt>
+                <c:pt idx="312">
+                  <c:v>6373</c:v>
+                </c:pt>
+                <c:pt idx="313">
+                  <c:v>6464</c:v>
+                </c:pt>
+                <c:pt idx="314">
+                  <c:v>6560</c:v>
+                </c:pt>
+                <c:pt idx="315">
+                  <c:v>6617</c:v>
+                </c:pt>
+                <c:pt idx="316">
+                  <c:v>7001</c:v>
+                </c:pt>
+                <c:pt idx="317">
+                  <c:v>7552</c:v>
+                </c:pt>
+                <c:pt idx="318">
+                  <c:v>8966</c:v>
+                </c:pt>
+                <c:pt idx="319">
+                  <c:v>10366</c:v>
+                </c:pt>
+                <c:pt idx="320">
+                  <c:v>10673</c:v>
+                </c:pt>
+                <c:pt idx="321">
+                  <c:v>10782</c:v>
+                </c:pt>
+                <c:pt idx="322">
+                  <c:v>10756</c:v>
+                </c:pt>
+                <c:pt idx="323">
+                  <c:v>10862</c:v>
+                </c:pt>
+                <c:pt idx="324">
+                  <c:v>10810</c:v>
+                </c:pt>
+                <c:pt idx="325">
+                  <c:v>10985</c:v>
+                </c:pt>
+                <c:pt idx="326">
+                  <c:v>11301</c:v>
+                </c:pt>
+                <c:pt idx="327">
+                  <c:v>11315</c:v>
+                </c:pt>
+                <c:pt idx="328">
+                  <c:v>11304</c:v>
+                </c:pt>
+                <c:pt idx="329">
+                  <c:v>11769</c:v>
+                </c:pt>
+                <c:pt idx="330">
+                  <c:v>11645</c:v>
+                </c:pt>
+                <c:pt idx="331">
+                  <c:v>11418</c:v>
+                </c:pt>
+                <c:pt idx="332">
+                  <c:v>10559</c:v>
+                </c:pt>
+                <c:pt idx="333">
+                  <c:v>10677</c:v>
+                </c:pt>
+                <c:pt idx="334">
+                  <c:v>10584</c:v>
+                </c:pt>
+                <c:pt idx="335">
+                  <c:v>10575</c:v>
+                </c:pt>
+                <c:pt idx="336">
+                  <c:v>10147</c:v>
+                </c:pt>
+                <c:pt idx="337">
+                  <c:v>10380</c:v>
+                </c:pt>
+                <c:pt idx="338">
+                  <c:v>10759</c:v>
+                </c:pt>
+                <c:pt idx="339">
+                  <c:v>11457</c:v>
+                </c:pt>
+                <c:pt idx="340">
+                  <c:v>11238</c:v>
+                </c:pt>
+                <c:pt idx="341">
+                  <c:v>11134</c:v>
+                </c:pt>
+                <c:pt idx="342">
+                  <c:v>11061</c:v>
+                </c:pt>
+                <c:pt idx="343">
+                  <c:v>11252</c:v>
+                </c:pt>
+                <c:pt idx="344">
+                  <c:v>10816</c:v>
+                </c:pt>
+                <c:pt idx="345">
+                  <c:v>10696</c:v>
+                </c:pt>
+                <c:pt idx="346">
+                  <c:v>10458</c:v>
+                </c:pt>
+                <c:pt idx="347">
+                  <c:v>10295</c:v>
+                </c:pt>
+                <c:pt idx="348">
+                  <c:v>10281</c:v>
+                </c:pt>
+                <c:pt idx="349">
+                  <c:v>10293</c:v>
+                </c:pt>
+                <c:pt idx="350">
+                  <c:v>10137</c:v>
+                </c:pt>
+                <c:pt idx="351">
+                  <c:v>10256</c:v>
+                </c:pt>
+                <c:pt idx="352">
+                  <c:v>9861</c:v>
+                </c:pt>
+                <c:pt idx="353">
+                  <c:v>9773</c:v>
+                </c:pt>
+                <c:pt idx="354">
+                  <c:v>9475</c:v>
+                </c:pt>
+                <c:pt idx="355">
+                  <c:v>9181</c:v>
+                </c:pt>
+                <c:pt idx="356">
+                  <c:v>9163</c:v>
+                </c:pt>
+                <c:pt idx="357">
+                  <c:v>8919</c:v>
+                </c:pt>
+                <c:pt idx="358">
+                  <c:v>8559</c:v>
+                </c:pt>
+                <c:pt idx="359">
+                  <c:v>8499</c:v>
+                </c:pt>
+                <c:pt idx="360">
+                  <c:v>8427</c:v>
+                </c:pt>
+                <c:pt idx="361">
+                  <c:v>8573</c:v>
+                </c:pt>
+                <c:pt idx="362">
+                  <c:v>8904</c:v>
+                </c:pt>
+                <c:pt idx="363">
+                  <c:v>8938</c:v>
+                </c:pt>
+                <c:pt idx="364">
+                  <c:v>9021</c:v>
+                </c:pt>
+                <c:pt idx="365">
+                  <c:v>9133</c:v>
+                </c:pt>
+                <c:pt idx="366">
+                  <c:v>9296</c:v>
+                </c:pt>
+                <c:pt idx="367">
+                  <c:v>9366</c:v>
+                </c:pt>
+                <c:pt idx="368">
+                  <c:v>9406</c:v>
+                </c:pt>
+                <c:pt idx="369">
+                  <c:v>9386</c:v>
+                </c:pt>
+                <c:pt idx="370">
+                  <c:v>9460</c:v>
+                </c:pt>
+                <c:pt idx="371">
+                  <c:v>9188</c:v>
+                </c:pt>
+                <c:pt idx="372">
+                  <c:v>9425</c:v>
+                </c:pt>
+                <c:pt idx="373">
+                  <c:v>9475</c:v>
+                </c:pt>
+                <c:pt idx="374">
+                  <c:v>9686</c:v>
+                </c:pt>
+                <c:pt idx="375">
+                  <c:v>10060</c:v>
+                </c:pt>
+                <c:pt idx="376">
+                  <c:v>10301</c:v>
+                </c:pt>
+                <c:pt idx="377">
+                  <c:v>10466</c:v>
+                </c:pt>
+                <c:pt idx="378">
+                  <c:v>11308</c:v>
+                </c:pt>
+                <c:pt idx="379">
+                  <c:v>11564</c:v>
+                </c:pt>
+                <c:pt idx="380">
+                  <c:v>11888</c:v>
+                </c:pt>
+                <c:pt idx="381">
+                  <c:v>12266</c:v>
+                </c:pt>
+                <c:pt idx="382">
+                  <c:v>12492</c:v>
+                </c:pt>
+                <c:pt idx="383">
+                  <c:v>12749</c:v>
+                </c:pt>
+                <c:pt idx="384">
+                  <c:v>12897</c:v>
+                </c:pt>
+                <c:pt idx="385">
+                  <c:v>13129</c:v>
+                </c:pt>
+                <c:pt idx="386">
+                  <c:v>13472</c:v>
+                </c:pt>
+                <c:pt idx="387">
+                  <c:v>13899</c:v>
+                </c:pt>
+                <c:pt idx="388">
+                  <c:v>14321</c:v>
+                </c:pt>
+                <c:pt idx="389">
+                  <c:v>14704</c:v>
+                </c:pt>
+                <c:pt idx="390">
+                  <c:v>14763</c:v>
+                </c:pt>
+                <c:pt idx="391">
+                  <c:v>14694</c:v>
+                </c:pt>
+                <c:pt idx="392">
+                  <c:v>15160</c:v>
+                </c:pt>
+                <c:pt idx="393">
+                  <c:v>15510</c:v>
+                </c:pt>
+                <c:pt idx="394">
+                  <c:v>15646</c:v>
+                </c:pt>
+                <c:pt idx="395">
+                  <c:v>16049</c:v>
+                </c:pt>
+                <c:pt idx="396">
+                  <c:v>16062</c:v>
+                </c:pt>
+                <c:pt idx="397">
+                  <c:v>16253</c:v>
+                </c:pt>
+                <c:pt idx="398">
+                  <c:v>16317</c:v>
+                </c:pt>
+                <c:pt idx="399">
+                  <c:v>16377</c:v>
+                </c:pt>
+                <c:pt idx="400">
+                  <c:v>16773</c:v>
+                </c:pt>
+                <c:pt idx="401">
+                  <c:v>17933</c:v>
+                </c:pt>
+                <c:pt idx="402">
+                  <c:v>17258</c:v>
+                </c:pt>
+                <c:pt idx="403">
+                  <c:v>15672</c:v>
+                </c:pt>
+                <c:pt idx="404">
+                  <c:v>15329</c:v>
+                </c:pt>
+                <c:pt idx="405">
+                  <c:v>15247</c:v>
+                </c:pt>
+                <c:pt idx="406">
+                  <c:v>15452</c:v>
+                </c:pt>
+                <c:pt idx="407">
+                  <c:v>15216</c:v>
+                </c:pt>
+                <c:pt idx="408">
+                  <c:v>14421</c:v>
+                </c:pt>
+                <c:pt idx="409">
+                  <c:v>14984</c:v>
+                </c:pt>
+                <c:pt idx="410">
+                  <c:v>16453</c:v>
+                </c:pt>
+                <c:pt idx="411">
+                  <c:v>16591</c:v>
+                </c:pt>
+                <c:pt idx="412">
+                  <c:v>16685</c:v>
+                </c:pt>
+                <c:pt idx="413">
+                  <c:v>16057</c:v>
+                </c:pt>
+                <c:pt idx="414">
+                  <c:v>15667</c:v>
+                </c:pt>
+                <c:pt idx="415">
+                  <c:v>15247</c:v>
+                </c:pt>
+                <c:pt idx="416">
+                  <c:v>14859</c:v>
+                </c:pt>
+                <c:pt idx="417">
+                  <c:v>14921</c:v>
+                </c:pt>
+                <c:pt idx="418">
+                  <c:v>14669</c:v>
+                </c:pt>
+                <c:pt idx="419">
+                  <c:v>14494</c:v>
+                </c:pt>
+                <c:pt idx="420">
+                  <c:v>14588</c:v>
+                </c:pt>
+                <c:pt idx="421">
+                  <c:v>14350</c:v>
+                </c:pt>
+                <c:pt idx="422">
+                  <c:v>12807</c:v>
+                </c:pt>
+                <c:pt idx="423">
+                  <c:v>12784</c:v>
+                </c:pt>
+                <c:pt idx="424">
+                  <c:v>12573</c:v>
+                </c:pt>
+                <c:pt idx="425">
+                  <c:v>12586</c:v>
+                </c:pt>
+                <c:pt idx="426">
+                  <c:v>12562</c:v>
+                </c:pt>
+                <c:pt idx="427">
+                  <c:v>12409</c:v>
+                </c:pt>
+                <c:pt idx="428">
+                  <c:v>12394</c:v>
+                </c:pt>
+                <c:pt idx="429">
+                  <c:v>13487</c:v>
+                </c:pt>
+                <c:pt idx="430">
+                  <c:v>13164</c:v>
+                </c:pt>
+                <c:pt idx="431">
+                  <c:v>12887</c:v>
+                </c:pt>
+                <c:pt idx="432">
+                  <c:v>12721</c:v>
+                </c:pt>
+                <c:pt idx="433">
+                  <c:v>12612</c:v>
+                </c:pt>
+                <c:pt idx="434">
+                  <c:v>12251</c:v>
+                </c:pt>
+                <c:pt idx="435">
+                  <c:v>11853</c:v>
+                </c:pt>
+                <c:pt idx="436">
+                  <c:v>11646</c:v>
+                </c:pt>
+                <c:pt idx="437">
+                  <c:v>11496</c:v>
+                </c:pt>
+                <c:pt idx="438">
+                  <c:v>11320</c:v>
+                </c:pt>
+                <c:pt idx="439">
+                  <c:v>11386</c:v>
+                </c:pt>
+                <c:pt idx="440">
+                  <c:v>11391</c:v>
+                </c:pt>
+                <c:pt idx="441">
+                  <c:v>11513</c:v>
+                </c:pt>
+                <c:pt idx="442">
+                  <c:v>11719</c:v>
+                </c:pt>
+                <c:pt idx="443">
+                  <c:v>12030</c:v>
+                </c:pt>
+                <c:pt idx="444">
+                  <c:v>12232</c:v>
+                </c:pt>
+                <c:pt idx="445">
+                  <c:v>12573</c:v>
+                </c:pt>
+                <c:pt idx="446">
+                  <c:v>12825</c:v>
+                </c:pt>
+                <c:pt idx="447">
+                  <c:v>12942</c:v>
+                </c:pt>
+                <c:pt idx="448">
+                  <c:v>12865</c:v>
+                </c:pt>
+                <c:pt idx="449">
+                  <c:v>13025</c:v>
+                </c:pt>
+                <c:pt idx="450">
+                  <c:v>13351</c:v>
+                </c:pt>
+              </c:numCache>
+              <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart"/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3DFE-427E-955C-335705931F90}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
@@ -5885,1415 +7282,6 @@
                 </c:extLst>
               </c15:ser>
             </c15:filteredLineSeries>
-            <c15:filteredLineSeries>
-              <c15:ser>
-                <c:idx val="1"/>
-                <c:order val="1"/>
-                <c:tx>
-                  <c:strRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>daily_changes!$F$1</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:strCache>
-                      <c:ptCount val="1"/>
-                      <c:pt idx="0">
-                        <c:v>∆C(t)</c:v>
-                      </c:pt>
-                    </c:strCache>
-                  </c:strRef>
-                </c:tx>
-                <c:spPr>
-                  <a:ln w="31750" cap="rnd">
-                    <a:solidFill>
-                      <a:schemeClr val="accent2"/>
-                    </a:solidFill>
-                    <a:round/>
-                  </a:ln>
-                  <a:effectLst/>
-                </c:spPr>
-                <c:marker>
-                  <c:symbol val="none"/>
-                </c:marker>
-                <c:val>
-                  <c:numRef>
-                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
-                        <c15:formulaRef>
-                          <c15:sqref>daily_changes!$F$2:$F$452</c15:sqref>
-                        </c15:formulaRef>
-                      </c:ext>
-                    </c:extLst>
-                    <c:numCache>
-                      <c:formatCode>General</c:formatCode>
-                      <c:ptCount val="451"/>
-                      <c:pt idx="0">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="1">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="2">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="3">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="4">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="5">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="6">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="7">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="8">
-                        <c:v>0</c:v>
-                      </c:pt>
-                      <c:pt idx="9">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="10">
-                        <c:v>1</c:v>
-                      </c:pt>
-                      <c:pt idx="11">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="12">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="13">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="14">
-                        <c:v>2</c:v>
-                      </c:pt>
-                      <c:pt idx="15">
-                        <c:v>4</c:v>
-                      </c:pt>
-                      <c:pt idx="16">
-                        <c:v>5</c:v>
-                      </c:pt>
-                      <c:pt idx="17">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="18">
-                        <c:v>7</c:v>
-                      </c:pt>
-                      <c:pt idx="19">
-                        <c:v>17</c:v>
-                      </c:pt>
-                      <c:pt idx="20">
-                        <c:v>19</c:v>
-                      </c:pt>
-                      <c:pt idx="21">
-                        <c:v>21</c:v>
-                      </c:pt>
-                      <c:pt idx="22">
-                        <c:v>30</c:v>
-                      </c:pt>
-                      <c:pt idx="23">
-                        <c:v>35</c:v>
-                      </c:pt>
-                      <c:pt idx="24">
-                        <c:v>49</c:v>
-                      </c:pt>
-                      <c:pt idx="25">
-                        <c:v>56</c:v>
-                      </c:pt>
-                      <c:pt idx="26">
-                        <c:v>71</c:v>
-                      </c:pt>
-                      <c:pt idx="27">
-                        <c:v>85</c:v>
-                      </c:pt>
-                      <c:pt idx="28">
-                        <c:v>92</c:v>
-                      </c:pt>
-                      <c:pt idx="29">
-                        <c:v>89</c:v>
-                      </c:pt>
-                      <c:pt idx="30">
-                        <c:v>109</c:v>
-                      </c:pt>
-                      <c:pt idx="31">
-                        <c:v>118</c:v>
-                      </c:pt>
-                      <c:pt idx="32">
-                        <c:v>135</c:v>
-                      </c:pt>
-                      <c:pt idx="33">
-                        <c:v>117</c:v>
-                      </c:pt>
-                      <c:pt idx="34">
-                        <c:v>110</c:v>
-                      </c:pt>
-                      <c:pt idx="35">
-                        <c:v>218</c:v>
-                      </c:pt>
-                      <c:pt idx="36">
-                        <c:v>303</c:v>
-                      </c:pt>
-                      <c:pt idx="37">
-                        <c:v>351</c:v>
-                      </c:pt>
-                      <c:pt idx="38">
-                        <c:v>404</c:v>
-                      </c:pt>
-                      <c:pt idx="39">
-                        <c:v>437</c:v>
-                      </c:pt>
-                      <c:pt idx="40">
-                        <c:v>453</c:v>
-                      </c:pt>
-                      <c:pt idx="41">
-                        <c:v>478</c:v>
-                      </c:pt>
-                      <c:pt idx="42">
-                        <c:v>478</c:v>
-                      </c:pt>
-                      <c:pt idx="43">
-                        <c:v>532</c:v>
-                      </c:pt>
-                      <c:pt idx="44">
-                        <c:v>568</c:v>
-                      </c:pt>
-                      <c:pt idx="45">
-                        <c:v>595</c:v>
-                      </c:pt>
-                      <c:pt idx="46">
-                        <c:v>565</c:v>
-                      </c:pt>
-                      <c:pt idx="47">
-                        <c:v>591</c:v>
-                      </c:pt>
-                      <c:pt idx="48">
-                        <c:v>576</c:v>
-                      </c:pt>
-                      <c:pt idx="49">
-                        <c:v>527</c:v>
-                      </c:pt>
-                      <c:pt idx="50">
-                        <c:v>619</c:v>
-                      </c:pt>
-                      <c:pt idx="51">
-                        <c:v>584</c:v>
-                      </c:pt>
-                      <c:pt idx="52">
-                        <c:v>661</c:v>
-                      </c:pt>
-                      <c:pt idx="53">
-                        <c:v>782</c:v>
-                      </c:pt>
-                      <c:pt idx="54">
-                        <c:v>787</c:v>
-                      </c:pt>
-                      <c:pt idx="55">
-                        <c:v>812</c:v>
-                      </c:pt>
-                      <c:pt idx="56">
-                        <c:v>859</c:v>
-                      </c:pt>
-                      <c:pt idx="57">
-                        <c:v>696</c:v>
-                      </c:pt>
-                      <c:pt idx="58">
-                        <c:v>739</c:v>
-                      </c:pt>
-                      <c:pt idx="59">
-                        <c:v>712</c:v>
-                      </c:pt>
-                      <c:pt idx="60">
-                        <c:v>873</c:v>
-                      </c:pt>
-                      <c:pt idx="61">
-                        <c:v>921</c:v>
-                      </c:pt>
-                      <c:pt idx="62">
-                        <c:v>1017</c:v>
-                      </c:pt>
-                      <c:pt idx="63">
-                        <c:v>1237</c:v>
-                      </c:pt>
-                      <c:pt idx="64">
-                        <c:v>1463</c:v>
-                      </c:pt>
-                      <c:pt idx="65">
-                        <c:v>1708</c:v>
-                      </c:pt>
-                      <c:pt idx="66">
-                        <c:v>1793</c:v>
-                      </c:pt>
-                      <c:pt idx="67">
-                        <c:v>1596</c:v>
-                      </c:pt>
-                      <c:pt idx="68">
-                        <c:v>1580</c:v>
-                      </c:pt>
-                      <c:pt idx="69">
-                        <c:v>1499</c:v>
-                      </c:pt>
-                      <c:pt idx="70">
-                        <c:v>1430</c:v>
-                      </c:pt>
-                      <c:pt idx="71">
-                        <c:v>1671</c:v>
-                      </c:pt>
-                      <c:pt idx="72">
-                        <c:v>1604</c:v>
-                      </c:pt>
-                      <c:pt idx="73">
-                        <c:v>1637</c:v>
-                      </c:pt>
-                      <c:pt idx="74">
-                        <c:v>1891</c:v>
-                      </c:pt>
-                      <c:pt idx="75">
-                        <c:v>1953</c:v>
-                      </c:pt>
-                      <c:pt idx="76">
-                        <c:v>1992</c:v>
-                      </c:pt>
-                      <c:pt idx="77">
-                        <c:v>1952</c:v>
-                      </c:pt>
-                      <c:pt idx="78">
-                        <c:v>1892</c:v>
-                      </c:pt>
-                      <c:pt idx="79">
-                        <c:v>2051</c:v>
-                      </c:pt>
-                      <c:pt idx="80">
-                        <c:v>2364</c:v>
-                      </c:pt>
-                      <c:pt idx="81">
-                        <c:v>2396</c:v>
-                      </c:pt>
-                      <c:pt idx="82">
-                        <c:v>2414</c:v>
-                      </c:pt>
-                      <c:pt idx="83">
-                        <c:v>2419</c:v>
-                      </c:pt>
-                      <c:pt idx="84">
-                        <c:v>2611</c:v>
-                      </c:pt>
-                      <c:pt idx="85">
-                        <c:v>2680</c:v>
-                      </c:pt>
-                      <c:pt idx="86">
-                        <c:v>2779</c:v>
-                      </c:pt>
-                      <c:pt idx="87">
-                        <c:v>2642</c:v>
-                      </c:pt>
-                      <c:pt idx="88">
-                        <c:v>2768</c:v>
-                      </c:pt>
-                      <c:pt idx="89">
-                        <c:v>2831</c:v>
-                      </c:pt>
-                      <c:pt idx="90">
-                        <c:v>2937</c:v>
-                      </c:pt>
-                      <c:pt idx="91">
-                        <c:v>2860</c:v>
-                      </c:pt>
-                      <c:pt idx="92">
-                        <c:v>2803</c:v>
-                      </c:pt>
-                      <c:pt idx="93">
-                        <c:v>3161</c:v>
-                      </c:pt>
-                      <c:pt idx="94">
-                        <c:v>3526</c:v>
-                      </c:pt>
-                      <c:pt idx="95">
-                        <c:v>3798</c:v>
-                      </c:pt>
-                      <c:pt idx="96">
-                        <c:v>3934</c:v>
-                      </c:pt>
-                      <c:pt idx="97">
-                        <c:v>3953</c:v>
-                      </c:pt>
-                      <c:pt idx="98">
-                        <c:v>4611</c:v>
-                      </c:pt>
-                      <c:pt idx="99">
-                        <c:v>4857</c:v>
-                      </c:pt>
-                      <c:pt idx="100">
-                        <c:v>4762</c:v>
-                      </c:pt>
-                      <c:pt idx="101">
-                        <c:v>4716</c:v>
-                      </c:pt>
-                      <c:pt idx="102">
-                        <c:v>4772</c:v>
-                      </c:pt>
-                      <c:pt idx="103">
-                        <c:v>4768</c:v>
-                      </c:pt>
-                      <c:pt idx="104">
-                        <c:v>4757</c:v>
-                      </c:pt>
-                      <c:pt idx="105">
-                        <c:v>4549</c:v>
-                      </c:pt>
-                      <c:pt idx="106">
-                        <c:v>4690</c:v>
-                      </c:pt>
-                      <c:pt idx="107">
-                        <c:v>4760</c:v>
-                      </c:pt>
-                      <c:pt idx="108">
-                        <c:v>4762</c:v>
-                      </c:pt>
-                      <c:pt idx="109">
-                        <c:v>4618</c:v>
-                      </c:pt>
-                      <c:pt idx="110">
-                        <c:v>5018</c:v>
-                      </c:pt>
-                      <c:pt idx="111">
-                        <c:v>5267</c:v>
-                      </c:pt>
-                      <c:pt idx="112">
-                        <c:v>5735</c:v>
-                      </c:pt>
-                      <c:pt idx="113">
-                        <c:v>5029</c:v>
-                      </c:pt>
-                      <c:pt idx="114">
-                        <c:v>4301</c:v>
-                      </c:pt>
-                      <c:pt idx="115">
-                        <c:v>6251</c:v>
-                      </c:pt>
-                      <c:pt idx="116">
-                        <c:v>6131</c:v>
-                      </c:pt>
-                      <c:pt idx="117">
-                        <c:v>5855</c:v>
-                      </c:pt>
-                      <c:pt idx="118">
-                        <c:v>5788</c:v>
-                      </c:pt>
-                      <c:pt idx="119">
-                        <c:v>5599</c:v>
-                      </c:pt>
-                      <c:pt idx="120">
-                        <c:v>6758</c:v>
-                      </c:pt>
-                      <c:pt idx="121">
-                        <c:v>7994</c:v>
-                      </c:pt>
-                      <c:pt idx="122">
-                        <c:v>6693</c:v>
-                      </c:pt>
-                      <c:pt idx="123">
-                        <c:v>7113</c:v>
-                      </c:pt>
-                      <c:pt idx="124">
-                        <c:v>7507</c:v>
-                      </c:pt>
-                      <c:pt idx="125">
-                        <c:v>7596</c:v>
-                      </c:pt>
-                      <c:pt idx="126">
-                        <c:v>7415</c:v>
-                      </c:pt>
-                      <c:pt idx="127">
-                        <c:v>7302</c:v>
-                      </c:pt>
-                      <c:pt idx="128">
-                        <c:v>7656</c:v>
-                      </c:pt>
-                      <c:pt idx="129">
-                        <c:v>7456</c:v>
-                      </c:pt>
-                      <c:pt idx="130">
-                        <c:v>6707</c:v>
-                      </c:pt>
-                      <c:pt idx="131">
-                        <c:v>6920</c:v>
-                      </c:pt>
-                      <c:pt idx="132">
-                        <c:v>6846</c:v>
-                      </c:pt>
-                      <c:pt idx="133">
-                        <c:v>7333</c:v>
-                      </c:pt>
-                      <c:pt idx="134">
-                        <c:v>7347</c:v>
-                      </c:pt>
-                      <c:pt idx="135">
-                        <c:v>6791</c:v>
-                      </c:pt>
-                      <c:pt idx="136">
-                        <c:v>6915</c:v>
-                      </c:pt>
-                      <c:pt idx="137">
-                        <c:v>7766</c:v>
-                      </c:pt>
-                      <c:pt idx="138">
-                        <c:v>7403</c:v>
-                      </c:pt>
-                      <c:pt idx="139">
-                        <c:v>7362</c:v>
-                      </c:pt>
-                      <c:pt idx="140">
-                        <c:v>7700</c:v>
-                      </c:pt>
-                      <c:pt idx="141">
-                        <c:v>7402</c:v>
-                      </c:pt>
-                      <c:pt idx="142">
-                        <c:v>7476</c:v>
-                      </c:pt>
-                      <c:pt idx="143">
-                        <c:v>6901</c:v>
-                      </c:pt>
-                      <c:pt idx="144">
-                        <c:v>6448</c:v>
-                      </c:pt>
-                      <c:pt idx="145">
-                        <c:v>6150</c:v>
-                      </c:pt>
-                      <c:pt idx="146">
-                        <c:v>5975</c:v>
-                      </c:pt>
-                      <c:pt idx="147">
-                        <c:v>5152</c:v>
-                      </c:pt>
-                      <c:pt idx="148">
-                        <c:v>6610</c:v>
-                      </c:pt>
-                      <c:pt idx="149">
-                        <c:v>7137</c:v>
-                      </c:pt>
-                      <c:pt idx="150">
-                        <c:v>7972</c:v>
-                      </c:pt>
-                      <c:pt idx="151">
-                        <c:v>9636</c:v>
-                      </c:pt>
-                      <c:pt idx="152">
-                        <c:v>9848</c:v>
-                      </c:pt>
-                      <c:pt idx="153">
-                        <c:v>10174</c:v>
-                      </c:pt>
-                      <c:pt idx="154">
-                        <c:v>9284</c:v>
-                      </c:pt>
-                      <c:pt idx="155">
-                        <c:v>10679</c:v>
-                      </c:pt>
-                      <c:pt idx="156">
-                        <c:v>11000</c:v>
-                      </c:pt>
-                      <c:pt idx="157">
-                        <c:v>11298</c:v>
-                      </c:pt>
-                      <c:pt idx="158">
-                        <c:v>10405</c:v>
-                      </c:pt>
-                      <c:pt idx="159">
-                        <c:v>10672</c:v>
-                      </c:pt>
-                      <c:pt idx="160">
-                        <c:v>10366</c:v>
-                      </c:pt>
-                      <c:pt idx="161">
-                        <c:v>12562</c:v>
-                      </c:pt>
-                      <c:pt idx="162">
-                        <c:v>10153</c:v>
-                      </c:pt>
-                      <c:pt idx="163">
-                        <c:v>9952</c:v>
-                      </c:pt>
-                      <c:pt idx="164">
-                        <c:v>9439</c:v>
-                      </c:pt>
-                      <c:pt idx="165">
-                        <c:v>9916</c:v>
-                      </c:pt>
-                      <c:pt idx="166">
-                        <c:v>9777</c:v>
-                      </c:pt>
-                      <c:pt idx="167">
-                        <c:v>9742</c:v>
-                      </c:pt>
-                      <c:pt idx="168">
-                        <c:v>9139</c:v>
-                      </c:pt>
-                      <c:pt idx="169">
-                        <c:v>9988</c:v>
-                      </c:pt>
-                      <c:pt idx="170">
-                        <c:v>10826</c:v>
-                      </c:pt>
-                      <c:pt idx="171">
-                        <c:v>11106</c:v>
-                      </c:pt>
-                      <c:pt idx="172">
-                        <c:v>10828</c:v>
-                      </c:pt>
-                      <c:pt idx="173">
-                        <c:v>10338</c:v>
-                      </c:pt>
-                      <c:pt idx="174">
-                        <c:v>10607</c:v>
-                      </c:pt>
-                      <c:pt idx="175">
-                        <c:v>10281</c:v>
-                      </c:pt>
-                      <c:pt idx="176">
-                        <c:v>9457</c:v>
-                      </c:pt>
-                      <c:pt idx="177">
-                        <c:v>8053</c:v>
-                      </c:pt>
-                      <c:pt idx="178">
-                        <c:v>7120</c:v>
-                      </c:pt>
-                      <c:pt idx="179">
-                        <c:v>7388</c:v>
-                      </c:pt>
-                      <c:pt idx="180">
-                        <c:v>7805</c:v>
-                      </c:pt>
-                      <c:pt idx="181">
-                        <c:v>7688</c:v>
-                      </c:pt>
-                      <c:pt idx="182">
-                        <c:v>7734</c:v>
-                      </c:pt>
-                      <c:pt idx="183">
-                        <c:v>7823</c:v>
-                      </c:pt>
-                      <c:pt idx="184">
-                        <c:v>7661</c:v>
-                      </c:pt>
-                      <c:pt idx="185">
-                        <c:v>8607</c:v>
-                      </c:pt>
-                      <c:pt idx="186">
-                        <c:v>7454</c:v>
-                      </c:pt>
-                      <c:pt idx="187">
-                        <c:v>7039</c:v>
-                      </c:pt>
-                      <c:pt idx="188">
-                        <c:v>6837</c:v>
-                      </c:pt>
-                      <c:pt idx="189">
-                        <c:v>6958</c:v>
-                      </c:pt>
-                      <c:pt idx="190">
-                        <c:v>7171</c:v>
-                      </c:pt>
-                      <c:pt idx="191">
-                        <c:v>7646</c:v>
-                      </c:pt>
-                      <c:pt idx="192">
-                        <c:v>6972</c:v>
-                      </c:pt>
-                      <c:pt idx="193">
-                        <c:v>7380</c:v>
-                      </c:pt>
-                      <c:pt idx="194">
-                        <c:v>7474</c:v>
-                      </c:pt>
-                      <c:pt idx="195">
-                        <c:v>7570</c:v>
-                      </c:pt>
-                      <c:pt idx="196">
-                        <c:v>6344</c:v>
-                      </c:pt>
-                      <c:pt idx="197">
-                        <c:v>5749</c:v>
-                      </c:pt>
-                      <c:pt idx="198">
-                        <c:v>5254</c:v>
-                      </c:pt>
-                      <c:pt idx="199">
-                        <c:v>5399</c:v>
-                      </c:pt>
-                      <c:pt idx="200">
-                        <c:v>5372</c:v>
-                      </c:pt>
-                      <c:pt idx="201">
-                        <c:v>5219</c:v>
-                      </c:pt>
-                      <c:pt idx="202">
-                        <c:v>5146</c:v>
-                      </c:pt>
-                      <c:pt idx="203">
-                        <c:v>6070</c:v>
-                      </c:pt>
-                      <c:pt idx="204">
-                        <c:v>6122</c:v>
-                      </c:pt>
-                      <c:pt idx="205">
-                        <c:v>6010</c:v>
-                      </c:pt>
-                      <c:pt idx="206">
-                        <c:v>5960</c:v>
-                      </c:pt>
-                      <c:pt idx="207">
-                        <c:v>5855</c:v>
-                      </c:pt>
-                      <c:pt idx="208">
-                        <c:v>6149</c:v>
-                      </c:pt>
-                      <c:pt idx="209">
-                        <c:v>6283</c:v>
-                      </c:pt>
-                      <c:pt idx="210">
-                        <c:v>6307</c:v>
-                      </c:pt>
-                      <c:pt idx="211">
-                        <c:v>6078</c:v>
-                      </c:pt>
-                      <c:pt idx="212">
-                        <c:v>5917</c:v>
-                      </c:pt>
-                      <c:pt idx="213">
-                        <c:v>5770</c:v>
-                      </c:pt>
-                      <c:pt idx="214">
-                        <c:v>5602</c:v>
-                      </c:pt>
-                      <c:pt idx="215">
-                        <c:v>5277</c:v>
-                      </c:pt>
-                      <c:pt idx="216">
-                        <c:v>5116</c:v>
-                      </c:pt>
-                      <c:pt idx="217">
-                        <c:v>4871</c:v>
-                      </c:pt>
-                      <c:pt idx="218">
-                        <c:v>4808</c:v>
-                      </c:pt>
-                      <c:pt idx="219">
-                        <c:v>4784</c:v>
-                      </c:pt>
-                      <c:pt idx="220">
-                        <c:v>4630</c:v>
-                      </c:pt>
-                      <c:pt idx="221">
-                        <c:v>4649</c:v>
-                      </c:pt>
-                      <c:pt idx="222">
-                        <c:v>4524</c:v>
-                      </c:pt>
-                      <c:pt idx="223">
-                        <c:v>4491</c:v>
-                      </c:pt>
-                      <c:pt idx="224">
-                        <c:v>4474</c:v>
-                      </c:pt>
-                      <c:pt idx="225">
-                        <c:v>4447</c:v>
-                      </c:pt>
-                      <c:pt idx="226">
-                        <c:v>4383</c:v>
-                      </c:pt>
-                      <c:pt idx="227">
-                        <c:v>4408</c:v>
-                      </c:pt>
-                      <c:pt idx="228">
-                        <c:v>4484</c:v>
-                      </c:pt>
-                      <c:pt idx="229">
-                        <c:v>4823</c:v>
-                      </c:pt>
-                      <c:pt idx="230">
-                        <c:v>4824</c:v>
-                      </c:pt>
-                      <c:pt idx="231">
-                        <c:v>4027</c:v>
-                      </c:pt>
-                      <c:pt idx="232">
-                        <c:v>4044</c:v>
-                      </c:pt>
-                      <c:pt idx="233">
-                        <c:v>4173</c:v>
-                      </c:pt>
-                      <c:pt idx="234">
-                        <c:v>4150</c:v>
-                      </c:pt>
-                      <c:pt idx="235">
-                        <c:v>3974</c:v>
-                      </c:pt>
-                      <c:pt idx="236">
-                        <c:v>3706</c:v>
-                      </c:pt>
-                      <c:pt idx="237">
-                        <c:v>3671</c:v>
-                      </c:pt>
-                      <c:pt idx="238">
-                        <c:v>4276</c:v>
-                      </c:pt>
-                      <c:pt idx="239">
-                        <c:v>4029</c:v>
-                      </c:pt>
-                      <c:pt idx="240">
-                        <c:v>3618</c:v>
-                      </c:pt>
-                      <c:pt idx="241">
-                        <c:v>3772</c:v>
-                      </c:pt>
-                      <c:pt idx="242">
-                        <c:v>3803</c:v>
-                      </c:pt>
-                      <c:pt idx="243">
-                        <c:v>4054</c:v>
-                      </c:pt>
-                      <c:pt idx="244">
-                        <c:v>4115</c:v>
-                      </c:pt>
-                      <c:pt idx="245">
-                        <c:v>4178</c:v>
-                      </c:pt>
-                      <c:pt idx="246">
-                        <c:v>4332</c:v>
-                      </c:pt>
-                      <c:pt idx="247">
-                        <c:v>4560</c:v>
-                      </c:pt>
-                      <c:pt idx="248">
-                        <c:v>4307</c:v>
-                      </c:pt>
-                      <c:pt idx="249">
-                        <c:v>3839</c:v>
-                      </c:pt>
-                      <c:pt idx="250">
-                        <c:v>3595</c:v>
-                      </c:pt>
-                      <c:pt idx="251">
-                        <c:v>3565</c:v>
-                      </c:pt>
-                      <c:pt idx="252">
-                        <c:v>2905</c:v>
-                      </c:pt>
-                      <c:pt idx="253">
-                        <c:v>2817</c:v>
-                      </c:pt>
-                      <c:pt idx="254">
-                        <c:v>2439</c:v>
-                      </c:pt>
-                      <c:pt idx="255">
-                        <c:v>1735</c:v>
-                      </c:pt>
-                      <c:pt idx="256">
-                        <c:v>1401</c:v>
-                      </c:pt>
-                      <c:pt idx="257">
-                        <c:v>1256</c:v>
-                      </c:pt>
-                      <c:pt idx="258">
-                        <c:v>1163</c:v>
-                      </c:pt>
-                      <c:pt idx="259">
-                        <c:v>1056</c:v>
-                      </c:pt>
-                      <c:pt idx="260">
-                        <c:v>3939</c:v>
-                      </c:pt>
-                      <c:pt idx="261">
-                        <c:v>4388</c:v>
-                      </c:pt>
-                      <c:pt idx="262">
-                        <c:v>5264</c:v>
-                      </c:pt>
-                      <c:pt idx="263">
-                        <c:v>5927</c:v>
-                      </c:pt>
-                      <c:pt idx="264">
-                        <c:v>6101</c:v>
-                      </c:pt>
-                      <c:pt idx="265">
-                        <c:v>6206</c:v>
-                      </c:pt>
-                      <c:pt idx="266">
-                        <c:v>7448</c:v>
-                      </c:pt>
-                      <c:pt idx="267">
-                        <c:v>4803</c:v>
-                      </c:pt>
-                      <c:pt idx="268">
-                        <c:v>4948</c:v>
-                      </c:pt>
-                      <c:pt idx="269">
-                        <c:v>5367</c:v>
-                      </c:pt>
-                      <c:pt idx="270">
-                        <c:v>5430</c:v>
-                      </c:pt>
-                      <c:pt idx="271">
-                        <c:v>5850</c:v>
-                      </c:pt>
-                      <c:pt idx="272">
-                        <c:v>5893</c:v>
-                      </c:pt>
-                      <c:pt idx="273">
-                        <c:v>5396</c:v>
-                      </c:pt>
-                      <c:pt idx="274">
-                        <c:v>5750</c:v>
-                      </c:pt>
-                      <c:pt idx="275">
-                        <c:v>5425</c:v>
-                      </c:pt>
-                      <c:pt idx="276">
-                        <c:v>4748</c:v>
-                      </c:pt>
-                      <c:pt idx="277">
-                        <c:v>4666</c:v>
-                      </c:pt>
-                      <c:pt idx="278">
-                        <c:v>4412</c:v>
-                      </c:pt>
-                      <c:pt idx="279">
-                        <c:v>4433</c:v>
-                      </c:pt>
-                      <c:pt idx="280">
-                        <c:v>4964</c:v>
-                      </c:pt>
-                      <c:pt idx="281">
-                        <c:v>4994</c:v>
-                      </c:pt>
-                      <c:pt idx="282">
-                        <c:v>5521</c:v>
-                      </c:pt>
-                      <c:pt idx="283">
-                        <c:v>6080</c:v>
-                      </c:pt>
-                      <c:pt idx="284">
-                        <c:v>6713</c:v>
-                      </c:pt>
-                      <c:pt idx="285">
-                        <c:v>6756</c:v>
-                      </c:pt>
-                      <c:pt idx="286">
-                        <c:v>6746</c:v>
-                      </c:pt>
-                      <c:pt idx="287">
-                        <c:v>6602</c:v>
-                      </c:pt>
-                      <c:pt idx="288">
-                        <c:v>6697</c:v>
-                      </c:pt>
-                      <c:pt idx="289">
-                        <c:v>6923</c:v>
-                      </c:pt>
-                      <c:pt idx="290">
-                        <c:v>7002</c:v>
-                      </c:pt>
-                      <c:pt idx="291">
-                        <c:v>6954</c:v>
-                      </c:pt>
-                      <c:pt idx="292">
-                        <c:v>6706</c:v>
-                      </c:pt>
-                      <c:pt idx="293">
-                        <c:v>6877</c:v>
-                      </c:pt>
-                      <c:pt idx="294">
-                        <c:v>6375</c:v>
-                      </c:pt>
-                      <c:pt idx="295">
-                        <c:v>4978</c:v>
-                      </c:pt>
-                      <c:pt idx="296">
-                        <c:v>6480</c:v>
-                      </c:pt>
-                      <c:pt idx="297">
-                        <c:v>6642</c:v>
-                      </c:pt>
-                      <c:pt idx="298">
-                        <c:v>7191</c:v>
-                      </c:pt>
-                      <c:pt idx="299">
-                        <c:v>7057</c:v>
-                      </c:pt>
-                      <c:pt idx="300">
-                        <c:v>7290</c:v>
-                      </c:pt>
-                      <c:pt idx="301">
-                        <c:v>8190</c:v>
-                      </c:pt>
-                      <c:pt idx="302">
-                        <c:v>9673</c:v>
-                      </c:pt>
-                      <c:pt idx="303">
-                        <c:v>8109</c:v>
-                      </c:pt>
-                      <c:pt idx="304">
-                        <c:v>7205</c:v>
-                      </c:pt>
-                      <c:pt idx="305">
-                        <c:v>5606</c:v>
-                      </c:pt>
-                      <c:pt idx="306">
-                        <c:v>6011</c:v>
-                      </c:pt>
-                      <c:pt idx="307">
-                        <c:v>5673</c:v>
-                      </c:pt>
-                      <c:pt idx="308">
-                        <c:v>5925</c:v>
-                      </c:pt>
-                      <c:pt idx="309">
-                        <c:v>6134</c:v>
-                      </c:pt>
-                      <c:pt idx="310">
-                        <c:v>6258</c:v>
-                      </c:pt>
-                      <c:pt idx="311">
-                        <c:v>6301</c:v>
-                      </c:pt>
-                      <c:pt idx="312">
-                        <c:v>6373</c:v>
-                      </c:pt>
-                      <c:pt idx="313">
-                        <c:v>6464</c:v>
-                      </c:pt>
-                      <c:pt idx="314">
-                        <c:v>6560</c:v>
-                      </c:pt>
-                      <c:pt idx="315">
-                        <c:v>6617</c:v>
-                      </c:pt>
-                      <c:pt idx="316">
-                        <c:v>7001</c:v>
-                      </c:pt>
-                      <c:pt idx="317">
-                        <c:v>7552</c:v>
-                      </c:pt>
-                      <c:pt idx="318">
-                        <c:v>8966</c:v>
-                      </c:pt>
-                      <c:pt idx="319">
-                        <c:v>10366</c:v>
-                      </c:pt>
-                      <c:pt idx="320">
-                        <c:v>10673</c:v>
-                      </c:pt>
-                      <c:pt idx="321">
-                        <c:v>10782</c:v>
-                      </c:pt>
-                      <c:pt idx="322">
-                        <c:v>10756</c:v>
-                      </c:pt>
-                      <c:pt idx="323">
-                        <c:v>10862</c:v>
-                      </c:pt>
-                      <c:pt idx="324">
-                        <c:v>10810</c:v>
-                      </c:pt>
-                      <c:pt idx="325">
-                        <c:v>10985</c:v>
-                      </c:pt>
-                      <c:pt idx="326">
-                        <c:v>11301</c:v>
-                      </c:pt>
-                      <c:pt idx="327">
-                        <c:v>11315</c:v>
-                      </c:pt>
-                      <c:pt idx="328">
-                        <c:v>11304</c:v>
-                      </c:pt>
-                      <c:pt idx="329">
-                        <c:v>11769</c:v>
-                      </c:pt>
-                      <c:pt idx="330">
-                        <c:v>11645</c:v>
-                      </c:pt>
-                      <c:pt idx="331">
-                        <c:v>11418</c:v>
-                      </c:pt>
-                      <c:pt idx="332">
-                        <c:v>10559</c:v>
-                      </c:pt>
-                      <c:pt idx="333">
-                        <c:v>10677</c:v>
-                      </c:pt>
-                      <c:pt idx="334">
-                        <c:v>10584</c:v>
-                      </c:pt>
-                      <c:pt idx="335">
-                        <c:v>10575</c:v>
-                      </c:pt>
-                      <c:pt idx="336">
-                        <c:v>10147</c:v>
-                      </c:pt>
-                      <c:pt idx="337">
-                        <c:v>10380</c:v>
-                      </c:pt>
-                      <c:pt idx="338">
-                        <c:v>10759</c:v>
-                      </c:pt>
-                      <c:pt idx="339">
-                        <c:v>11457</c:v>
-                      </c:pt>
-                      <c:pt idx="340">
-                        <c:v>11238</c:v>
-                      </c:pt>
-                      <c:pt idx="341">
-                        <c:v>11134</c:v>
-                      </c:pt>
-                      <c:pt idx="342">
-                        <c:v>11061</c:v>
-                      </c:pt>
-                      <c:pt idx="343">
-                        <c:v>11252</c:v>
-                      </c:pt>
-                      <c:pt idx="344">
-                        <c:v>10816</c:v>
-                      </c:pt>
-                      <c:pt idx="345">
-                        <c:v>10696</c:v>
-                      </c:pt>
-                      <c:pt idx="346">
-                        <c:v>10458</c:v>
-                      </c:pt>
-                      <c:pt idx="347">
-                        <c:v>10295</c:v>
-                      </c:pt>
-                      <c:pt idx="348">
-                        <c:v>10281</c:v>
-                      </c:pt>
-                      <c:pt idx="349">
-                        <c:v>10293</c:v>
-                      </c:pt>
-                      <c:pt idx="350">
-                        <c:v>10137</c:v>
-                      </c:pt>
-                      <c:pt idx="351">
-                        <c:v>10256</c:v>
-                      </c:pt>
-                      <c:pt idx="352">
-                        <c:v>9861</c:v>
-                      </c:pt>
-                      <c:pt idx="353">
-                        <c:v>9773</c:v>
-                      </c:pt>
-                      <c:pt idx="354">
-                        <c:v>9475</c:v>
-                      </c:pt>
-                      <c:pt idx="355">
-                        <c:v>9181</c:v>
-                      </c:pt>
-                      <c:pt idx="356">
-                        <c:v>9163</c:v>
-                      </c:pt>
-                      <c:pt idx="357">
-                        <c:v>8919</c:v>
-                      </c:pt>
-                      <c:pt idx="358">
-                        <c:v>8559</c:v>
-                      </c:pt>
-                      <c:pt idx="359">
-                        <c:v>8499</c:v>
-                      </c:pt>
-                      <c:pt idx="360">
-                        <c:v>8427</c:v>
-                      </c:pt>
-                      <c:pt idx="361">
-                        <c:v>8573</c:v>
-                      </c:pt>
-                      <c:pt idx="362">
-                        <c:v>8904</c:v>
-                      </c:pt>
-                      <c:pt idx="363">
-                        <c:v>8938</c:v>
-                      </c:pt>
-                      <c:pt idx="364">
-                        <c:v>9021</c:v>
-                      </c:pt>
-                      <c:pt idx="365">
-                        <c:v>9133</c:v>
-                      </c:pt>
-                      <c:pt idx="366">
-                        <c:v>9296</c:v>
-                      </c:pt>
-                      <c:pt idx="367">
-                        <c:v>9366</c:v>
-                      </c:pt>
-                      <c:pt idx="368">
-                        <c:v>9406</c:v>
-                      </c:pt>
-                      <c:pt idx="369">
-                        <c:v>9386</c:v>
-                      </c:pt>
-                      <c:pt idx="370">
-                        <c:v>9460</c:v>
-                      </c:pt>
-                      <c:pt idx="371">
-                        <c:v>9188</c:v>
-                      </c:pt>
-                      <c:pt idx="372">
-                        <c:v>9425</c:v>
-                      </c:pt>
-                      <c:pt idx="373">
-                        <c:v>9475</c:v>
-                      </c:pt>
-                      <c:pt idx="374">
-                        <c:v>9686</c:v>
-                      </c:pt>
-                      <c:pt idx="375">
-                        <c:v>10060</c:v>
-                      </c:pt>
-                      <c:pt idx="376">
-                        <c:v>10301</c:v>
-                      </c:pt>
-                      <c:pt idx="377">
-                        <c:v>10466</c:v>
-                      </c:pt>
-                      <c:pt idx="378">
-                        <c:v>11308</c:v>
-                      </c:pt>
-                      <c:pt idx="379">
-                        <c:v>11564</c:v>
-                      </c:pt>
-                      <c:pt idx="380">
-                        <c:v>11888</c:v>
-                      </c:pt>
-                      <c:pt idx="381">
-                        <c:v>12266</c:v>
-                      </c:pt>
-                      <c:pt idx="382">
-                        <c:v>12492</c:v>
-                      </c:pt>
-                      <c:pt idx="383">
-                        <c:v>12749</c:v>
-                      </c:pt>
-                      <c:pt idx="384">
-                        <c:v>12897</c:v>
-                      </c:pt>
-                      <c:pt idx="385">
-                        <c:v>13129</c:v>
-                      </c:pt>
-                      <c:pt idx="386">
-                        <c:v>13472</c:v>
-                      </c:pt>
-                      <c:pt idx="387">
-                        <c:v>13899</c:v>
-                      </c:pt>
-                      <c:pt idx="388">
-                        <c:v>14321</c:v>
-                      </c:pt>
-                      <c:pt idx="389">
-                        <c:v>14704</c:v>
-                      </c:pt>
-                      <c:pt idx="390">
-                        <c:v>14763</c:v>
-                      </c:pt>
-                      <c:pt idx="391">
-                        <c:v>14694</c:v>
-                      </c:pt>
-                      <c:pt idx="392">
-                        <c:v>15160</c:v>
-                      </c:pt>
-                      <c:pt idx="393">
-                        <c:v>15510</c:v>
-                      </c:pt>
-                      <c:pt idx="394">
-                        <c:v>15646</c:v>
-                      </c:pt>
-                      <c:pt idx="395">
-                        <c:v>16049</c:v>
-                      </c:pt>
-                      <c:pt idx="396">
-                        <c:v>16062</c:v>
-                      </c:pt>
-                      <c:pt idx="397">
-                        <c:v>16253</c:v>
-                      </c:pt>
-                      <c:pt idx="398">
-                        <c:v>16317</c:v>
-                      </c:pt>
-                      <c:pt idx="399">
-                        <c:v>16377</c:v>
-                      </c:pt>
-                      <c:pt idx="400">
-                        <c:v>16773</c:v>
-                      </c:pt>
-                      <c:pt idx="401">
-                        <c:v>17933</c:v>
-                      </c:pt>
-                      <c:pt idx="402">
-                        <c:v>17258</c:v>
-                      </c:pt>
-                      <c:pt idx="403">
-                        <c:v>15672</c:v>
-                      </c:pt>
-                      <c:pt idx="404">
-                        <c:v>15329</c:v>
-                      </c:pt>
-                      <c:pt idx="405">
-                        <c:v>15247</c:v>
-                      </c:pt>
-                      <c:pt idx="406">
-                        <c:v>15452</c:v>
-                      </c:pt>
-                      <c:pt idx="407">
-                        <c:v>15216</c:v>
-                      </c:pt>
-                      <c:pt idx="408">
-                        <c:v>14421</c:v>
-                      </c:pt>
-                      <c:pt idx="409">
-                        <c:v>14984</c:v>
-                      </c:pt>
-                      <c:pt idx="410">
-                        <c:v>16453</c:v>
-                      </c:pt>
-                      <c:pt idx="411">
-                        <c:v>16591</c:v>
-                      </c:pt>
-                      <c:pt idx="412">
-                        <c:v>16685</c:v>
-                      </c:pt>
-                      <c:pt idx="413">
-                        <c:v>16057</c:v>
-                      </c:pt>
-                      <c:pt idx="414">
-                        <c:v>15667</c:v>
-                      </c:pt>
-                      <c:pt idx="415">
-                        <c:v>15247</c:v>
-                      </c:pt>
-                      <c:pt idx="416">
-                        <c:v>14859</c:v>
-                      </c:pt>
-                      <c:pt idx="417">
-                        <c:v>14921</c:v>
-                      </c:pt>
-                      <c:pt idx="418">
-                        <c:v>14669</c:v>
-                      </c:pt>
-                      <c:pt idx="419">
-                        <c:v>14494</c:v>
-                      </c:pt>
-                      <c:pt idx="420">
-                        <c:v>14588</c:v>
-                      </c:pt>
-                      <c:pt idx="421">
-                        <c:v>14350</c:v>
-                      </c:pt>
-                      <c:pt idx="422">
-                        <c:v>12807</c:v>
-                      </c:pt>
-                      <c:pt idx="423">
-                        <c:v>12784</c:v>
-                      </c:pt>
-                      <c:pt idx="424">
-                        <c:v>12573</c:v>
-                      </c:pt>
-                      <c:pt idx="425">
-                        <c:v>12586</c:v>
-                      </c:pt>
-                      <c:pt idx="426">
-                        <c:v>12562</c:v>
-                      </c:pt>
-                      <c:pt idx="427">
-                        <c:v>12409</c:v>
-                      </c:pt>
-                      <c:pt idx="428">
-                        <c:v>12394</c:v>
-                      </c:pt>
-                      <c:pt idx="429">
-                        <c:v>13487</c:v>
-                      </c:pt>
-                      <c:pt idx="430">
-                        <c:v>13164</c:v>
-                      </c:pt>
-                      <c:pt idx="431">
-                        <c:v>12887</c:v>
-                      </c:pt>
-                      <c:pt idx="432">
-                        <c:v>12721</c:v>
-                      </c:pt>
-                      <c:pt idx="433">
-                        <c:v>12612</c:v>
-                      </c:pt>
-                      <c:pt idx="434">
-                        <c:v>12251</c:v>
-                      </c:pt>
-                      <c:pt idx="435">
-                        <c:v>11853</c:v>
-                      </c:pt>
-                      <c:pt idx="436">
-                        <c:v>11646</c:v>
-                      </c:pt>
-                      <c:pt idx="437">
-                        <c:v>11496</c:v>
-                      </c:pt>
-                      <c:pt idx="438">
-                        <c:v>11320</c:v>
-                      </c:pt>
-                      <c:pt idx="439">
-                        <c:v>11386</c:v>
-                      </c:pt>
-                      <c:pt idx="440">
-                        <c:v>11391</c:v>
-                      </c:pt>
-                      <c:pt idx="441">
-                        <c:v>11513</c:v>
-                      </c:pt>
-                      <c:pt idx="442">
-                        <c:v>11719</c:v>
-                      </c:pt>
-                      <c:pt idx="443">
-                        <c:v>12030</c:v>
-                      </c:pt>
-                      <c:pt idx="444">
-                        <c:v>12232</c:v>
-                      </c:pt>
-                      <c:pt idx="445">
-                        <c:v>12573</c:v>
-                      </c:pt>
-                      <c:pt idx="446">
-                        <c:v>12825</c:v>
-                      </c:pt>
-                      <c:pt idx="447">
-                        <c:v>12942</c:v>
-                      </c:pt>
-                      <c:pt idx="448">
-                        <c:v>12865</c:v>
-                      </c:pt>
-                      <c:pt idx="449">
-                        <c:v>13025</c:v>
-                      </c:pt>
-                      <c:pt idx="450">
-                        <c:v>13351</c:v>
-                      </c:pt>
-                    </c:numCache>
-                  </c:numRef>
-                </c:val>
-                <c:smooth val="0"/>
-                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
-                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-                    <c16:uniqueId val="{00000001-3DFE-427E-955C-335705931F90}"/>
-                  </c:ext>
-                </c:extLst>
-              </c15:ser>
-            </c15:filteredLineSeries>
           </c:ext>
         </c:extLst>
       </c:lineChart>
@@ -7491,37 +7479,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -16399,7 +16357,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5D8998D-AD55-4463-BC89-DF91B734F996}">
   <dimension ref="A1:K452"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
@@ -32250,9 +32208,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{29AB0DAB-7BA8-4CD5-9366-3DC25D1E98DB}">
   <dimension ref="A1:I452"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -45388,9 +45344,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A2416008-25B5-4A17-BA72-B8F072D2CFC5}">
   <dimension ref="A1:I452"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K42" sqref="K42"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>

</xml_diff>